<commit_message>
removed duplicate file and updated file
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_fullrun_hbrown_09.27.19.xlsx
+++ b/fastqFiles/fastq_fullrun_hbrown_09.27.19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/fastqFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B62B646-1350-6C4A-A2EC-117F38126D60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFA410E-3C12-5C48-A826-FC3167C67D7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="13200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13060" yWindow="460" windowWidth="16380" windowHeight="13200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="65">
   <si>
     <t>libraryDate</t>
   </si>
@@ -133,6 +133,93 @@
   </si>
   <si>
     <t>Brent_2c-19_GTAC_59_SIC_Index2_6_AGTTATG_GACCTTGT_S20_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>07.22.19</t>
+  </si>
+  <si>
+    <t>HighOutput</t>
+  </si>
+  <si>
+    <t>Brent_2d-1_GTAC_41_SIC_Index2_7_TTGCCCC_GAGTTGGT_S28_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-2_GTAC_42_SIC_Index2_7_ACTCCAA_GAGTTGGT_S29_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-3_GTAC_43_SIC_Index2_7_TGTGCCA_GAGTTGGT_S30_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-4_GTAC_44_SIC_Index2_7_AACGGAG_GAGTTGGT_S31_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-5_GTAC_45_SIC_Index2_7_GATAGTT_GAGTTGGT_S32_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-6_GTAC_46_SIC_Index2_7_GGTGAAT_GAGTTGGT_S33_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-7_GTAC_47_SIC_Index2_7_ATGTTCT_GAGTTGGT_S34_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-8_GTAC_48_SIC_Index2_7_GTAAAAA_GAGTTGGT_S35_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-9_GTAC_49_SIC_Index2_7_GTCTGAT_GAGTTGGT_S36_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-10_GTAC_50_SIC_Index2_7_CAATATC_GAGTTGGT_S37_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-11_GTAC_51_SIC_Index2_7_CTCCCGA_GAGTTGGT_S38_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-12_GTAC_52_SIC_Index2_7_GCCGTTT_GAGTTGGT_S39_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-13_GTAC_53_SIC_Index2_7_TAGGTAA_GAGTTGGT_S40_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-14_GTAC_54_SIC_Index2_7_TCGAGAT_GAGTTGGT_S41_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-15_GTAC_55_SIC_Index2_7_CATTTAG_GAGTTGGT_S42_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-16_GTAC_56_SIC_Index2_7_TCCGGGA_GAGTTGGT_S43_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-17_GTAC_57_SIC_Index2_7_CGAAAGT_GAGTTGGT_S44_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-18_GTAC_58_SIC_Index2_7_GCCTCCC_GAGTTGGT_S45_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-19_GTAC_59_SIC_Index2_7_AGTTATG_GAGTTGGT_S46_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-20_GTAC_60_SIC_Index2_7_CTGCAAT_GAGTTGGT_S47_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-21_GTAC_61_SIC_Index2_7_CAAGCCG_GAGTTGGT_S48_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Brent_2d-22_GTAC_62_SIC_Index2_7_GGGTCAA_GAGTTGGT_S49_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-23_GTAC_63_SIC_Index2_7_GCAACGC_GAGTTGGT_S50_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-24_GTAC_64_SIC_Index2_7_TGATTAC_GAGTTGGT_S51_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-25_GTAC_65_SIC_Index2_7_TGCTGGG_GAGTTGGT_S52_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2d-26_GTAC_66_SIC_Index2_7_GACACAG_GAGTTGGT_S53_R1_001.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -195,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -211,6 +298,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -527,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z20"/>
+  <dimension ref="A1:Z46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D20"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1130,7 +1223,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1165,7 +1258,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1200,7 +1293,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1235,7 +1328,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1268,6 +1361,891 @@
       </c>
       <c r="L20" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>3906</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="9">
+        <v>156</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0.87324960960960996</v>
+      </c>
+      <c r="K21" s="10">
+        <v>6628739</v>
+      </c>
+      <c r="L21" t="s">
+        <v>38</v>
+      </c>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>3906</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22">
+        <v>205</v>
+      </c>
+      <c r="J22">
+        <v>0.76053908722374797</v>
+      </c>
+      <c r="K22">
+        <v>7246147</v>
+      </c>
+      <c r="L22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>3906</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23">
+        <v>99.5</v>
+      </c>
+      <c r="J23">
+        <v>1.0090817038258</v>
+      </c>
+      <c r="K23">
+        <v>7033022</v>
+      </c>
+      <c r="L23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>3906</v>
+      </c>
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24">
+        <v>153</v>
+      </c>
+      <c r="J24">
+        <v>1.1201545454545501</v>
+      </c>
+      <c r="K24">
+        <v>5830709</v>
+      </c>
+      <c r="L24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>3906</v>
+      </c>
+      <c r="F25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25">
+        <v>24.9</v>
+      </c>
+      <c r="J25">
+        <v>0.56412458412144095</v>
+      </c>
+      <c r="K25">
+        <v>6602748</v>
+      </c>
+      <c r="L25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+      <c r="D26">
+        <v>3906</v>
+      </c>
+      <c r="F26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26">
+        <v>47.1</v>
+      </c>
+      <c r="J26">
+        <v>0.90301100846207605</v>
+      </c>
+      <c r="K26">
+        <v>5364357</v>
+      </c>
+      <c r="L26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
+      </c>
+      <c r="D27">
+        <v>3906</v>
+      </c>
+      <c r="F27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27">
+        <v>5.72</v>
+      </c>
+      <c r="J27">
+        <v>1.5565167657938099</v>
+      </c>
+      <c r="K27">
+        <v>8176651</v>
+      </c>
+      <c r="L27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28">
+        <v>3906</v>
+      </c>
+      <c r="F28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" t="s">
+        <v>37</v>
+      </c>
+      <c r="H28" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28">
+        <v>20.9</v>
+      </c>
+      <c r="J28">
+        <v>0.66275518076408102</v>
+      </c>
+      <c r="K28">
+        <v>7535848</v>
+      </c>
+      <c r="L28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29">
+        <v>9</v>
+      </c>
+      <c r="D29">
+        <v>3906</v>
+      </c>
+      <c r="F29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29">
+        <v>272</v>
+      </c>
+      <c r="J29">
+        <v>0.86933369207772804</v>
+      </c>
+      <c r="K29">
+        <v>7591733</v>
+      </c>
+      <c r="L29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>3906</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30">
+        <v>181</v>
+      </c>
+      <c r="J30">
+        <v>1.0020403859407301</v>
+      </c>
+      <c r="K30">
+        <v>6284042</v>
+      </c>
+      <c r="L30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31">
+        <v>11</v>
+      </c>
+      <c r="D31">
+        <v>3906</v>
+      </c>
+      <c r="F31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31">
+        <v>211</v>
+      </c>
+      <c r="J31">
+        <v>0.80257260746567305</v>
+      </c>
+      <c r="K31">
+        <v>7185205</v>
+      </c>
+      <c r="L31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32">
+        <v>12</v>
+      </c>
+      <c r="D32">
+        <v>3906</v>
+      </c>
+      <c r="F32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32">
+        <v>225</v>
+      </c>
+      <c r="J32">
+        <v>0.96472462469934495</v>
+      </c>
+      <c r="K32">
+        <v>5686830</v>
+      </c>
+      <c r="L32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33">
+        <v>13</v>
+      </c>
+      <c r="D33">
+        <v>3906</v>
+      </c>
+      <c r="F33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" t="s">
+        <v>37</v>
+      </c>
+      <c r="H33" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33">
+        <v>205</v>
+      </c>
+      <c r="J33">
+        <v>0.65641562076749405</v>
+      </c>
+      <c r="K33">
+        <v>6371816</v>
+      </c>
+      <c r="L33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34">
+        <v>14</v>
+      </c>
+      <c r="D34">
+        <v>3906</v>
+      </c>
+      <c r="F34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" t="s">
+        <v>37</v>
+      </c>
+      <c r="H34" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34">
+        <v>67</v>
+      </c>
+      <c r="J34">
+        <v>0.84357869238858496</v>
+      </c>
+      <c r="K34">
+        <v>5108335</v>
+      </c>
+      <c r="L34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35">
+        <v>15</v>
+      </c>
+      <c r="D35">
+        <v>3906</v>
+      </c>
+      <c r="F35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" t="s">
+        <v>37</v>
+      </c>
+      <c r="H35" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35">
+        <v>188</v>
+      </c>
+      <c r="J35">
+        <v>0.94149377150026303</v>
+      </c>
+      <c r="K35">
+        <v>6319000</v>
+      </c>
+      <c r="L35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36">
+        <v>16</v>
+      </c>
+      <c r="D36">
+        <v>3906</v>
+      </c>
+      <c r="F36" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" t="s">
+        <v>37</v>
+      </c>
+      <c r="H36" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36">
+        <v>118</v>
+      </c>
+      <c r="J36">
+        <v>0.59074072117826304</v>
+      </c>
+      <c r="K36">
+        <v>7659797</v>
+      </c>
+      <c r="L36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37">
+        <v>17</v>
+      </c>
+      <c r="D37">
+        <v>3906</v>
+      </c>
+      <c r="F37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" t="s">
+        <v>37</v>
+      </c>
+      <c r="H37" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="L37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38">
+        <v>18</v>
+      </c>
+      <c r="D38">
+        <v>3906</v>
+      </c>
+      <c r="F38" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" t="s">
+        <v>37</v>
+      </c>
+      <c r="H38" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="J38">
+        <v>1.46411791805652</v>
+      </c>
+      <c r="K38">
+        <v>9800442</v>
+      </c>
+      <c r="L38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39">
+        <v>19</v>
+      </c>
+      <c r="D39">
+        <v>3906</v>
+      </c>
+      <c r="F39" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" t="s">
+        <v>37</v>
+      </c>
+      <c r="H39" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39">
+        <v>233</v>
+      </c>
+      <c r="J39">
+        <v>0.81677443999719102</v>
+      </c>
+      <c r="K39">
+        <v>6717693</v>
+      </c>
+      <c r="L39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40">
+        <v>20</v>
+      </c>
+      <c r="D40">
+        <v>3906</v>
+      </c>
+      <c r="F40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" t="s">
+        <v>37</v>
+      </c>
+      <c r="H40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40">
+        <v>253</v>
+      </c>
+      <c r="J40">
+        <v>0.84004512331636205</v>
+      </c>
+      <c r="K40">
+        <v>6649107</v>
+      </c>
+      <c r="L40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41">
+        <v>21</v>
+      </c>
+      <c r="D41">
+        <v>3906</v>
+      </c>
+      <c r="F41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" t="s">
+        <v>37</v>
+      </c>
+      <c r="H41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="L41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42">
+        <v>22</v>
+      </c>
+      <c r="D42">
+        <v>3906</v>
+      </c>
+      <c r="F42" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" t="s">
+        <v>37</v>
+      </c>
+      <c r="H42" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="J42" t="s">
+        <v>59</v>
+      </c>
+      <c r="L42" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43">
+        <v>23</v>
+      </c>
+      <c r="D43">
+        <v>3906</v>
+      </c>
+      <c r="F43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" t="s">
+        <v>37</v>
+      </c>
+      <c r="H43" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="L43" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44">
+        <v>24</v>
+      </c>
+      <c r="D44">
+        <v>3906</v>
+      </c>
+      <c r="F44" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" t="s">
+        <v>37</v>
+      </c>
+      <c r="H44" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44">
+        <v>0.317</v>
+      </c>
+      <c r="L44" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45">
+        <v>25</v>
+      </c>
+      <c r="D45">
+        <v>3906</v>
+      </c>
+      <c r="F45" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45" t="s">
+        <v>37</v>
+      </c>
+      <c r="H45" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45">
+        <v>233</v>
+      </c>
+      <c r="J45">
+        <v>0.84272304292700595</v>
+      </c>
+      <c r="K45">
+        <v>6395198</v>
+      </c>
+      <c r="L45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46">
+        <v>26</v>
+      </c>
+      <c r="D46">
+        <v>3906</v>
+      </c>
+      <c r="F46" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" t="s">
+        <v>37</v>
+      </c>
+      <c r="H46" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46">
+        <v>181</v>
+      </c>
+      <c r="J46">
+        <v>1.06065607076095</v>
+      </c>
+      <c r="K46">
+        <v>6850105</v>
+      </c>
+      <c r="L46" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>